<commit_message>
improving data, I hope
</commit_message>
<xml_diff>
--- a/ASAwards/AthenaSWANAwardList2012_201520160316.xlsx
+++ b/ASAwards/AthenaSWANAwardList2012_201520160316.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="1640" windowWidth="25040" windowHeight="14420"/>
+    <workbookView xWindow="360" yWindow="0" windowWidth="25040" windowHeight="14420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -558,9 +558,6 @@
     <t>Keele University, School of Physical &amp; Geographical Sciences</t>
   </si>
   <si>
-    <t>Kings College London, Centre of Human &amp; Aerospace Physiological Sciences (CHAPS)</t>
-  </si>
-  <si>
     <t>Newcastle University, School of Biomedical Sciences</t>
   </si>
   <si>
@@ -729,9 +726,6 @@
     <t>University of York, Department of Chemistry</t>
   </si>
   <si>
-    <t>King's College London, Division of Immunology, Infection and Inflammatory Diseases</t>
-  </si>
-  <si>
     <t>University College London, UCL Institute of Cardiovascular Science</t>
   </si>
   <si>
@@ -766,9 +760,6 @@
   </si>
   <si>
     <t>Imperial College London, Department of Physics</t>
-  </si>
-  <si>
-    <t>Queen's University Belfast, School of Geography, Archaeology and Palaeoecology</t>
   </si>
   <si>
     <t>Royal Holloway, Department of Physics</t>
@@ -1177,18 +1168,6 @@
     <t>Imperial College London – Institute of Clinical Sciences and MRC Clinical Sciences Centre</t>
   </si>
   <si>
-    <t>King's College London – Division of Palliative Care, Policy and Rehabilitation</t>
-  </si>
-  <si>
-    <t>King's College London – Division of Asthma, Allergy and Lung Biology</t>
-  </si>
-  <si>
-    <t>King's College London – Division of Imaging Sciences and Biomedical Engineering</t>
-  </si>
-  <si>
-    <t>King's College London – Faculty of Natural and Mathematical Sciences</t>
-  </si>
-  <si>
     <t>London School of Hygiene and Tropical Medicine – Faculty of Infectious and Tropical Diseases</t>
   </si>
   <si>
@@ -1321,15 +1300,6 @@
     <t>University of Cambridge</t>
   </si>
   <si>
-    <t>King's College London – Cardiovascular Division</t>
-  </si>
-  <si>
-    <t>King's College London – Division of Women’s Health</t>
-  </si>
-  <si>
-    <t>Queen's University Belfast – School of Pharmacy</t>
-  </si>
-  <si>
     <t>University College London – UCL Cancer Institute</t>
   </si>
   <si>
@@ -1432,9 +1402,6 @@
     <t>Heriot-Watt University</t>
   </si>
   <si>
-    <t>Kings College London</t>
-  </si>
-  <si>
     <t>Sheffield Hallam University</t>
   </si>
   <si>
@@ -1703,16 +1670,65 @@
   </si>
   <si>
     <t>School of Chemistry, University of Edinburgh</t>
+  </si>
+  <si>
+    <t>Queen’s University Belfast, School of Geography, Archaeology and Palaeoecology</t>
+  </si>
+  <si>
+    <t>Queen’s University Belfast – School of Pharmacy</t>
+  </si>
+  <si>
+    <t>King’s College London – Division of Asthma, Allergy and Lung Biology</t>
+  </si>
+  <si>
+    <t>King’s College London – Division of Imaging Sciences and Biomedical Engineering</t>
+  </si>
+  <si>
+    <t>King’s College London – Division of Palliative Care, Policy and Rehabilitation</t>
+  </si>
+  <si>
+    <t>King’s College London – Faculty of Natural and Mathematical Sciences</t>
+  </si>
+  <si>
+    <t>King’s College London, Centre of Human &amp; Aerospace Physiological Sciences (CHAPS)</t>
+  </si>
+  <si>
+    <t>King’s College London, Division of Immunology, Infection and Inflammatory Diseases</t>
+  </si>
+  <si>
+    <t>King’s College London – Cardiovascular Division</t>
+  </si>
+  <si>
+    <t>King’s College London – Division of Women’s Health</t>
+  </si>
+  <si>
+    <t>King’s College London</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1735,13 +1751,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2073,8 +2093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F566"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A509" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F182" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="F188" sqref="F188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2299,7 +2319,7 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>179</v>
+        <v>556</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2319,7 +2339,7 @@
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2339,7 +2359,7 @@
         <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2359,7 +2379,7 @@
         <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2379,7 +2399,7 @@
         <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2399,7 +2419,7 @@
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2419,7 +2439,7 @@
         <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2439,7 +2459,7 @@
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2459,7 +2479,7 @@
         <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2479,7 +2499,7 @@
         <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2499,7 +2519,7 @@
         <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2519,7 +2539,7 @@
         <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2539,7 +2559,7 @@
         <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2559,7 +2579,7 @@
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2579,7 +2599,7 @@
         <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2599,7 +2619,7 @@
         <v>15</v>
       </c>
       <c r="F26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2619,7 +2639,7 @@
         <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2639,7 +2659,7 @@
         <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2659,7 +2679,7 @@
         <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2679,7 +2699,7 @@
         <v>15</v>
       </c>
       <c r="F30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2699,7 +2719,7 @@
         <v>15</v>
       </c>
       <c r="F31" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2719,7 +2739,7 @@
         <v>15</v>
       </c>
       <c r="F32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2739,7 +2759,7 @@
         <v>15</v>
       </c>
       <c r="F33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2759,7 +2779,7 @@
         <v>15</v>
       </c>
       <c r="F34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2779,7 +2799,7 @@
         <v>15</v>
       </c>
       <c r="F35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2799,7 +2819,7 @@
         <v>15</v>
       </c>
       <c r="F36" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2819,7 +2839,7 @@
         <v>15</v>
       </c>
       <c r="F37" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2839,7 +2859,7 @@
         <v>15</v>
       </c>
       <c r="F38" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2859,7 +2879,7 @@
         <v>15</v>
       </c>
       <c r="F39" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2879,7 +2899,7 @@
         <v>15</v>
       </c>
       <c r="F40" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2899,7 +2919,7 @@
         <v>15</v>
       </c>
       <c r="F41" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2919,7 +2939,7 @@
         <v>15</v>
       </c>
       <c r="F42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2939,7 +2959,7 @@
         <v>15</v>
       </c>
       <c r="F43" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2959,7 +2979,7 @@
         <v>15</v>
       </c>
       <c r="F44" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2979,7 +2999,7 @@
         <v>15</v>
       </c>
       <c r="F45" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2999,7 +3019,7 @@
         <v>15</v>
       </c>
       <c r="F46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -3019,7 +3039,7 @@
         <v>15</v>
       </c>
       <c r="F47" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -3039,7 +3059,7 @@
         <v>15</v>
       </c>
       <c r="F48" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -3059,7 +3079,7 @@
         <v>15</v>
       </c>
       <c r="F49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -3079,7 +3099,7 @@
         <v>15</v>
       </c>
       <c r="F50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -3099,7 +3119,7 @@
         <v>15</v>
       </c>
       <c r="F51" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -3119,7 +3139,7 @@
         <v>15</v>
       </c>
       <c r="F52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -3139,7 +3159,7 @@
         <v>15</v>
       </c>
       <c r="F53" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -3159,7 +3179,7 @@
         <v>15</v>
       </c>
       <c r="F54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -3179,7 +3199,7 @@
         <v>15</v>
       </c>
       <c r="F55" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -3219,7 +3239,7 @@
         <v>15</v>
       </c>
       <c r="F57" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -3299,7 +3319,7 @@
         <v>15</v>
       </c>
       <c r="F61" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -3319,7 +3339,7 @@
         <v>15</v>
       </c>
       <c r="F62" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -3339,7 +3359,7 @@
         <v>15</v>
       </c>
       <c r="F63" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -3359,7 +3379,7 @@
         <v>15</v>
       </c>
       <c r="F64" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -3379,7 +3399,7 @@
         <v>15</v>
       </c>
       <c r="F65" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -3399,7 +3419,7 @@
         <v>15</v>
       </c>
       <c r="F66" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -3419,7 +3439,7 @@
         <v>15</v>
       </c>
       <c r="F67" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -3439,7 +3459,7 @@
         <v>15</v>
       </c>
       <c r="F68" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -3459,7 +3479,7 @@
         <v>15</v>
       </c>
       <c r="F69" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -3479,12 +3499,12 @@
         <v>15</v>
       </c>
       <c r="F70" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B71" t="s">
         <v>10</v>
@@ -3499,7 +3519,7 @@
         <v>15</v>
       </c>
       <c r="F71" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -3519,7 +3539,7 @@
         <v>15</v>
       </c>
       <c r="F72" t="s">
-        <v>236</v>
+        <v>557</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -3579,7 +3599,7 @@
         <v>15</v>
       </c>
       <c r="F75" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -3619,7 +3639,7 @@
         <v>15</v>
       </c>
       <c r="F77" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -3639,7 +3659,7 @@
         <v>15</v>
       </c>
       <c r="F78" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -3679,7 +3699,7 @@
         <v>15</v>
       </c>
       <c r="F80" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -3699,7 +3719,7 @@
         <v>15</v>
       </c>
       <c r="F81" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -3719,7 +3739,7 @@
         <v>15</v>
       </c>
       <c r="F82" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -3759,7 +3779,7 @@
         <v>15</v>
       </c>
       <c r="F84" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -3779,7 +3799,7 @@
         <v>15</v>
       </c>
       <c r="F85" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -3839,7 +3859,7 @@
         <v>15</v>
       </c>
       <c r="F88" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -3859,7 +3879,7 @@
         <v>15</v>
       </c>
       <c r="F89" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -3879,7 +3899,7 @@
         <v>15</v>
       </c>
       <c r="F90" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -3899,7 +3919,7 @@
         <v>15</v>
       </c>
       <c r="F91" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -3919,7 +3939,7 @@
         <v>15</v>
       </c>
       <c r="F92" t="s">
-        <v>249</v>
+        <v>550</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -3939,7 +3959,7 @@
         <v>15</v>
       </c>
       <c r="F93" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -3959,7 +3979,7 @@
         <v>15</v>
       </c>
       <c r="F94" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -3979,7 +3999,7 @@
         <v>15</v>
       </c>
       <c r="F95" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -3999,7 +4019,7 @@
         <v>15</v>
       </c>
       <c r="F96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -4019,7 +4039,7 @@
         <v>15</v>
       </c>
       <c r="F97" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -4039,7 +4059,7 @@
         <v>15</v>
       </c>
       <c r="F98" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -4059,7 +4079,7 @@
         <v>16</v>
       </c>
       <c r="F99" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -4079,7 +4099,7 @@
         <v>16</v>
       </c>
       <c r="F100" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -4099,7 +4119,7 @@
         <v>16</v>
       </c>
       <c r="F101" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -4119,7 +4139,7 @@
         <v>16</v>
       </c>
       <c r="F102" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -4139,7 +4159,7 @@
         <v>16</v>
       </c>
       <c r="F103" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -4159,7 +4179,7 @@
         <v>16</v>
       </c>
       <c r="F104" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -4179,7 +4199,7 @@
         <v>16</v>
       </c>
       <c r="F105" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -4199,7 +4219,7 @@
         <v>16</v>
       </c>
       <c r="F106" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -4219,7 +4239,7 @@
         <v>16</v>
       </c>
       <c r="F107" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -4239,7 +4259,7 @@
         <v>16</v>
       </c>
       <c r="F108" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -4259,7 +4279,7 @@
         <v>16</v>
       </c>
       <c r="F109" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -4279,7 +4299,7 @@
         <v>16</v>
       </c>
       <c r="F110" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -4299,7 +4319,7 @@
         <v>16</v>
       </c>
       <c r="F111" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -4319,7 +4339,7 @@
         <v>16</v>
       </c>
       <c r="F112" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -4339,7 +4359,7 @@
         <v>16</v>
       </c>
       <c r="F113" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -4359,7 +4379,7 @@
         <v>16</v>
       </c>
       <c r="F114" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -4379,7 +4399,7 @@
         <v>16</v>
       </c>
       <c r="F115" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -4399,7 +4419,7 @@
         <v>16</v>
       </c>
       <c r="F116" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -4419,7 +4439,7 @@
         <v>16</v>
       </c>
       <c r="F117" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -4439,7 +4459,7 @@
         <v>16</v>
       </c>
       <c r="F118" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -4459,7 +4479,7 @@
         <v>16</v>
       </c>
       <c r="F119" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -4479,7 +4499,7 @@
         <v>16</v>
       </c>
       <c r="F120" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -4499,7 +4519,7 @@
         <v>16</v>
       </c>
       <c r="F121" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -4519,7 +4539,7 @@
         <v>16</v>
       </c>
       <c r="F122" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -4539,7 +4559,7 @@
         <v>16</v>
       </c>
       <c r="F123" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -4559,7 +4579,7 @@
         <v>16</v>
       </c>
       <c r="F124" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -4579,7 +4599,7 @@
         <v>16</v>
       </c>
       <c r="F125" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -4599,7 +4619,7 @@
         <v>16</v>
       </c>
       <c r="F126" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -4619,7 +4639,7 @@
         <v>16</v>
       </c>
       <c r="F127" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -4639,7 +4659,7 @@
         <v>16</v>
       </c>
       <c r="F128" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -4659,7 +4679,7 @@
         <v>16</v>
       </c>
       <c r="F129" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -4679,7 +4699,7 @@
         <v>16</v>
       </c>
       <c r="F130" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -4699,7 +4719,7 @@
         <v>16</v>
       </c>
       <c r="F131" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -4719,7 +4739,7 @@
         <v>16</v>
       </c>
       <c r="F132" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -4739,7 +4759,7 @@
         <v>16</v>
       </c>
       <c r="F133" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -4759,7 +4779,7 @@
         <v>16</v>
       </c>
       <c r="F134" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -4779,7 +4799,7 @@
         <v>16</v>
       </c>
       <c r="F135" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -4799,7 +4819,7 @@
         <v>16</v>
       </c>
       <c r="F136" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -4819,7 +4839,7 @@
         <v>16</v>
       </c>
       <c r="F137" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -4839,7 +4859,7 @@
         <v>16</v>
       </c>
       <c r="F138" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="139" spans="1:6">
@@ -4859,7 +4879,7 @@
         <v>16</v>
       </c>
       <c r="F139" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -4879,7 +4899,7 @@
         <v>16</v>
       </c>
       <c r="F140" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -4899,7 +4919,7 @@
         <v>16</v>
       </c>
       <c r="F141" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="142" spans="1:6">
@@ -4919,7 +4939,7 @@
         <v>16</v>
       </c>
       <c r="F142" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -4939,7 +4959,7 @@
         <v>16</v>
       </c>
       <c r="F143" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -4959,7 +4979,7 @@
         <v>16</v>
       </c>
       <c r="F144" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -4979,7 +4999,7 @@
         <v>16</v>
       </c>
       <c r="F145" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -4999,7 +5019,7 @@
         <v>16</v>
       </c>
       <c r="F146" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -5019,7 +5039,7 @@
         <v>16</v>
       </c>
       <c r="F147" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -5039,7 +5059,7 @@
         <v>16</v>
       </c>
       <c r="F148" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -5059,7 +5079,7 @@
         <v>16</v>
       </c>
       <c r="F149" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -5079,7 +5099,7 @@
         <v>16</v>
       </c>
       <c r="F150" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="151" spans="1:6">
@@ -5099,7 +5119,7 @@
         <v>16</v>
       </c>
       <c r="F151" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="152" spans="1:6">
@@ -5119,7 +5139,7 @@
         <v>16</v>
       </c>
       <c r="F152" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="153" spans="1:6">
@@ -5139,7 +5159,7 @@
         <v>16</v>
       </c>
       <c r="F153" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="154" spans="1:6">
@@ -5159,7 +5179,7 @@
         <v>16</v>
       </c>
       <c r="F154" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="155" spans="1:6">
@@ -5179,7 +5199,7 @@
         <v>16</v>
       </c>
       <c r="F155" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="156" spans="1:6">
@@ -5199,7 +5219,7 @@
         <v>16</v>
       </c>
       <c r="F156" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="157" spans="1:6">
@@ -5219,7 +5239,7 @@
         <v>16</v>
       </c>
       <c r="F157" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="158" spans="1:6">
@@ -5239,7 +5259,7 @@
         <v>16</v>
       </c>
       <c r="F158" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="159" spans="1:6">
@@ -5259,7 +5279,7 @@
         <v>16</v>
       </c>
       <c r="F159" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="160" spans="1:6">
@@ -5279,7 +5299,7 @@
         <v>16</v>
       </c>
       <c r="F160" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="161" spans="1:6">
@@ -5299,7 +5319,7 @@
         <v>16</v>
       </c>
       <c r="F161" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="162" spans="1:6">
@@ -5319,7 +5339,7 @@
         <v>16</v>
       </c>
       <c r="F162" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="163" spans="1:6">
@@ -5339,7 +5359,7 @@
         <v>16</v>
       </c>
       <c r="F163" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="164" spans="1:6">
@@ -5359,7 +5379,7 @@
         <v>16</v>
       </c>
       <c r="F164" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="165" spans="1:6">
@@ -5379,7 +5399,7 @@
         <v>16</v>
       </c>
       <c r="F165" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="166" spans="1:6">
@@ -5399,7 +5419,7 @@
         <v>16</v>
       </c>
       <c r="F166" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="167" spans="1:6">
@@ -5419,7 +5439,7 @@
         <v>16</v>
       </c>
       <c r="F167" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="168" spans="1:6">
@@ -5439,7 +5459,7 @@
         <v>16</v>
       </c>
       <c r="F168" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="169" spans="1:6">
@@ -5459,7 +5479,7 @@
         <v>16</v>
       </c>
       <c r="F169" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="170" spans="1:6">
@@ -5479,7 +5499,7 @@
         <v>16</v>
       </c>
       <c r="F170" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="171" spans="1:6">
@@ -5499,7 +5519,7 @@
         <v>16</v>
       </c>
       <c r="F171" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="172" spans="1:6">
@@ -5519,7 +5539,7 @@
         <v>16</v>
       </c>
       <c r="F172" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="173" spans="1:6">
@@ -5539,7 +5559,7 @@
         <v>16</v>
       </c>
       <c r="F173" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="174" spans="1:6">
@@ -5559,7 +5579,7 @@
         <v>16</v>
       </c>
       <c r="F174" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="175" spans="1:6">
@@ -5579,7 +5599,7 @@
         <v>16</v>
       </c>
       <c r="F175" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="176" spans="1:6">
@@ -5599,7 +5619,7 @@
         <v>16</v>
       </c>
       <c r="F176" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="177" spans="1:6">
@@ -5619,7 +5639,7 @@
         <v>16</v>
       </c>
       <c r="F177" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="178" spans="1:6">
@@ -5639,7 +5659,7 @@
         <v>16</v>
       </c>
       <c r="F178" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="179" spans="1:6">
@@ -5659,7 +5679,7 @@
         <v>16</v>
       </c>
       <c r="F179" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="180" spans="1:6">
@@ -5679,7 +5699,7 @@
         <v>16</v>
       </c>
       <c r="F180" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="181" spans="1:6">
@@ -5699,7 +5719,7 @@
         <v>16</v>
       </c>
       <c r="F181" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="182" spans="1:6">
@@ -5719,7 +5739,7 @@
         <v>16</v>
       </c>
       <c r="F182" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="183" spans="1:6">
@@ -5739,7 +5759,7 @@
         <v>16</v>
       </c>
       <c r="F183" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="184" spans="1:6">
@@ -5759,7 +5779,7 @@
         <v>16</v>
       </c>
       <c r="F184" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="185" spans="1:6">
@@ -5779,7 +5799,7 @@
         <v>16</v>
       </c>
       <c r="F185" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="186" spans="1:6">
@@ -5799,7 +5819,7 @@
         <v>16</v>
       </c>
       <c r="F186" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="187" spans="1:6">
@@ -5819,7 +5839,7 @@
         <v>16</v>
       </c>
       <c r="F187" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="188" spans="1:6">
@@ -5839,7 +5859,7 @@
         <v>16</v>
       </c>
       <c r="F188" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="189" spans="1:6">
@@ -5859,7 +5879,7 @@
         <v>16</v>
       </c>
       <c r="F189" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="190" spans="1:6">
@@ -5879,7 +5899,7 @@
         <v>16</v>
       </c>
       <c r="F190" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="191" spans="1:6">
@@ -5899,7 +5919,7 @@
         <v>16</v>
       </c>
       <c r="F191" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="192" spans="1:6">
@@ -5919,7 +5939,7 @@
         <v>16</v>
       </c>
       <c r="F192" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="193" spans="1:6">
@@ -5939,7 +5959,7 @@
         <v>16</v>
       </c>
       <c r="F193" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="194" spans="1:6">
@@ -5959,7 +5979,7 @@
         <v>16</v>
       </c>
       <c r="F194" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="195" spans="1:6">
@@ -5979,7 +5999,7 @@
         <v>16</v>
       </c>
       <c r="F195" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="196" spans="1:6">
@@ -5999,7 +6019,7 @@
         <v>16</v>
       </c>
       <c r="F196" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="197" spans="1:6">
@@ -6019,7 +6039,7 @@
         <v>16</v>
       </c>
       <c r="F197" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="198" spans="1:6">
@@ -6039,7 +6059,7 @@
         <v>16</v>
       </c>
       <c r="F198" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="199" spans="1:6">
@@ -6059,7 +6079,7 @@
         <v>16</v>
       </c>
       <c r="F199" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="200" spans="1:6">
@@ -6079,7 +6099,7 @@
         <v>16</v>
       </c>
       <c r="F200" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="201" spans="1:6">
@@ -6099,7 +6119,7 @@
         <v>16</v>
       </c>
       <c r="F201" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="202" spans="1:6">
@@ -6119,7 +6139,7 @@
         <v>16</v>
       </c>
       <c r="F202" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="203" spans="1:6">
@@ -6139,7 +6159,7 @@
         <v>16</v>
       </c>
       <c r="F203" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="204" spans="1:6">
@@ -6159,7 +6179,7 @@
         <v>16</v>
       </c>
       <c r="F204" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="205" spans="1:6">
@@ -6179,7 +6199,7 @@
         <v>16</v>
       </c>
       <c r="F205" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="206" spans="1:6">
@@ -6199,7 +6219,7 @@
         <v>16</v>
       </c>
       <c r="F206" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="207" spans="1:6">
@@ -6219,7 +6239,7 @@
         <v>16</v>
       </c>
       <c r="F207" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="208" spans="1:6">
@@ -6239,7 +6259,7 @@
         <v>16</v>
       </c>
       <c r="F208" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="209" spans="1:6">
@@ -6259,7 +6279,7 @@
         <v>16</v>
       </c>
       <c r="F209" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="210" spans="1:6">
@@ -6279,7 +6299,7 @@
         <v>16</v>
       </c>
       <c r="F210" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="211" spans="1:6">
@@ -6299,7 +6319,7 @@
         <v>16</v>
       </c>
       <c r="F211" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="212" spans="1:6">
@@ -6319,7 +6339,7 @@
         <v>15</v>
       </c>
       <c r="F212" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="213" spans="1:6">
@@ -6339,7 +6359,7 @@
         <v>15</v>
       </c>
       <c r="F213" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="214" spans="1:6">
@@ -6359,7 +6379,7 @@
         <v>15</v>
       </c>
       <c r="F214" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="215" spans="1:6">
@@ -6379,7 +6399,7 @@
         <v>15</v>
       </c>
       <c r="F215" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="216" spans="1:6">
@@ -6399,7 +6419,7 @@
         <v>15</v>
       </c>
       <c r="F216" t="s">
-        <v>386</v>
+        <v>552</v>
       </c>
     </row>
     <row r="217" spans="1:6">
@@ -6419,7 +6439,7 @@
         <v>15</v>
       </c>
       <c r="F217" t="s">
-        <v>387</v>
+        <v>553</v>
       </c>
     </row>
     <row r="218" spans="1:6">
@@ -6439,7 +6459,7 @@
         <v>15</v>
       </c>
       <c r="F218" t="s">
-        <v>385</v>
+        <v>554</v>
       </c>
     </row>
     <row r="219" spans="1:6">
@@ -6459,7 +6479,7 @@
         <v>15</v>
       </c>
       <c r="F219" t="s">
-        <v>388</v>
+        <v>555</v>
       </c>
     </row>
     <row r="220" spans="1:6">
@@ -6479,7 +6499,7 @@
         <v>15</v>
       </c>
       <c r="F220" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="221" spans="1:6">
@@ -6499,7 +6519,7 @@
         <v>15</v>
       </c>
       <c r="F221" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="222" spans="1:6">
@@ -6519,7 +6539,7 @@
         <v>15</v>
       </c>
       <c r="F222" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="223" spans="1:6">
@@ -6539,7 +6559,7 @@
         <v>15</v>
       </c>
       <c r="F223" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="224" spans="1:6">
@@ -6559,7 +6579,7 @@
         <v>15</v>
       </c>
       <c r="F224" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
     </row>
     <row r="225" spans="1:6">
@@ -6579,7 +6599,7 @@
         <v>15</v>
       </c>
       <c r="F225" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="226" spans="1:6">
@@ -6599,7 +6619,7 @@
         <v>15</v>
       </c>
       <c r="F226" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="227" spans="1:6">
@@ -6619,7 +6639,7 @@
         <v>15</v>
       </c>
       <c r="F227" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
     <row r="228" spans="1:6">
@@ -6639,7 +6659,7 @@
         <v>15</v>
       </c>
       <c r="F228" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
     </row>
     <row r="229" spans="1:6">
@@ -6659,7 +6679,7 @@
         <v>15</v>
       </c>
       <c r="F229" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
     </row>
     <row r="230" spans="1:6">
@@ -6679,7 +6699,7 @@
         <v>15</v>
       </c>
       <c r="F230" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
     </row>
     <row r="231" spans="1:6">
@@ -6699,7 +6719,7 @@
         <v>15</v>
       </c>
       <c r="F231" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="232" spans="1:6">
@@ -6719,7 +6739,7 @@
         <v>15</v>
       </c>
       <c r="F232" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
     </row>
     <row r="233" spans="1:6">
@@ -6739,7 +6759,7 @@
         <v>15</v>
       </c>
       <c r="F233" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="234" spans="1:6">
@@ -6759,7 +6779,7 @@
         <v>15</v>
       </c>
       <c r="F234" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
     </row>
     <row r="235" spans="1:6">
@@ -6779,7 +6799,7 @@
         <v>15</v>
       </c>
       <c r="F235" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
     </row>
     <row r="236" spans="1:6">
@@ -6799,7 +6819,7 @@
         <v>15</v>
       </c>
       <c r="F236" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
     <row r="237" spans="1:6">
@@ -6819,7 +6839,7 @@
         <v>15</v>
       </c>
       <c r="F237" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
     </row>
     <row r="238" spans="1:6">
@@ -6839,7 +6859,7 @@
         <v>15</v>
       </c>
       <c r="F238" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
     </row>
     <row r="239" spans="1:6">
@@ -6859,7 +6879,7 @@
         <v>15</v>
       </c>
       <c r="F239" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
     </row>
     <row r="240" spans="1:6">
@@ -6879,7 +6899,7 @@
         <v>15</v>
       </c>
       <c r="F240" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
     </row>
     <row r="241" spans="1:6">
@@ -6899,7 +6919,7 @@
         <v>15</v>
       </c>
       <c r="F241" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
     </row>
     <row r="242" spans="1:6">
@@ -6919,7 +6939,7 @@
         <v>15</v>
       </c>
       <c r="F242" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
     </row>
     <row r="243" spans="1:6">
@@ -6939,7 +6959,7 @@
         <v>15</v>
       </c>
       <c r="F243" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
     </row>
     <row r="244" spans="1:6">
@@ -6959,7 +6979,7 @@
         <v>15</v>
       </c>
       <c r="F244" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
     </row>
     <row r="245" spans="1:6">
@@ -6979,7 +6999,7 @@
         <v>15</v>
       </c>
       <c r="F245" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
     </row>
     <row r="246" spans="1:6">
@@ -6999,7 +7019,7 @@
         <v>15</v>
       </c>
       <c r="F246" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
     </row>
     <row r="247" spans="1:6">
@@ -7019,7 +7039,7 @@
         <v>15</v>
       </c>
       <c r="F247" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
     </row>
     <row r="248" spans="1:6">
@@ -7039,7 +7059,7 @@
         <v>15</v>
       </c>
       <c r="F248" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
     </row>
     <row r="249" spans="1:6">
@@ -7059,7 +7079,7 @@
         <v>15</v>
       </c>
       <c r="F249" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
     </row>
     <row r="250" spans="1:6">
@@ -7079,7 +7099,7 @@
         <v>15</v>
       </c>
       <c r="F250" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
     </row>
     <row r="251" spans="1:6">
@@ -7099,7 +7119,7 @@
         <v>15</v>
       </c>
       <c r="F251" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
     </row>
     <row r="252" spans="1:6">
@@ -7119,7 +7139,7 @@
         <v>15</v>
       </c>
       <c r="F252" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="253" spans="1:6">
@@ -7139,7 +7159,7 @@
         <v>15</v>
       </c>
       <c r="F253" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
     </row>
     <row r="254" spans="1:6">
@@ -7159,7 +7179,7 @@
         <v>15</v>
       </c>
       <c r="F254" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
     </row>
     <row r="255" spans="1:6">
@@ -7179,7 +7199,7 @@
         <v>15</v>
       </c>
       <c r="F255" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
     </row>
     <row r="256" spans="1:6">
@@ -7199,7 +7219,7 @@
         <v>15</v>
       </c>
       <c r="F256" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
     </row>
     <row r="257" spans="1:6">
@@ -7219,7 +7239,7 @@
         <v>15</v>
       </c>
       <c r="F257" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="258" spans="1:6">
@@ -7239,7 +7259,7 @@
         <v>15</v>
       </c>
       <c r="F258" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
     </row>
     <row r="259" spans="1:6">
@@ -7259,7 +7279,7 @@
         <v>15</v>
       </c>
       <c r="F259" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
     </row>
     <row r="260" spans="1:6">
@@ -7279,7 +7299,7 @@
         <v>15</v>
       </c>
       <c r="F260" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
     </row>
     <row r="261" spans="1:6">
@@ -7299,7 +7319,7 @@
         <v>15</v>
       </c>
       <c r="F261" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="262" spans="1:6">
@@ -7319,7 +7339,7 @@
         <v>15</v>
       </c>
       <c r="F262" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
     </row>
     <row r="263" spans="1:6">
@@ -7339,7 +7359,7 @@
         <v>15</v>
       </c>
       <c r="F263" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="264" spans="1:6">
@@ -7359,7 +7379,7 @@
         <v>15</v>
       </c>
       <c r="F264" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="265" spans="1:6">
@@ -7379,7 +7399,7 @@
         <v>15</v>
       </c>
       <c r="F265" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="266" spans="1:6">
@@ -7399,7 +7419,7 @@
         <v>15</v>
       </c>
       <c r="F266" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="267" spans="1:6">
@@ -7419,7 +7439,7 @@
         <v>15</v>
       </c>
       <c r="F267" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="268" spans="1:6">
@@ -7439,7 +7459,7 @@
         <v>15</v>
       </c>
       <c r="F268" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="269" spans="1:6">
@@ -7459,7 +7479,7 @@
         <v>15</v>
       </c>
       <c r="F269" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="270" spans="1:6">
@@ -7479,7 +7499,7 @@
         <v>15</v>
       </c>
       <c r="F270" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="271" spans="1:6">
@@ -7499,7 +7519,7 @@
         <v>15</v>
       </c>
       <c r="F271" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="272" spans="1:6">
@@ -7519,7 +7539,7 @@
         <v>15</v>
       </c>
       <c r="F272" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="273" spans="1:6">
@@ -7539,7 +7559,7 @@
         <v>15</v>
       </c>
       <c r="F273" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="274" spans="1:6">
@@ -7559,7 +7579,7 @@
         <v>15</v>
       </c>
       <c r="F274" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="275" spans="1:6">
@@ -7579,7 +7599,7 @@
         <v>15</v>
       </c>
       <c r="F275" t="s">
-        <v>433</v>
+        <v>558</v>
       </c>
     </row>
     <row r="276" spans="1:6">
@@ -7599,7 +7619,7 @@
         <v>15</v>
       </c>
       <c r="F276" t="s">
-        <v>434</v>
+        <v>559</v>
       </c>
     </row>
     <row r="277" spans="1:6">
@@ -7619,7 +7639,7 @@
         <v>15</v>
       </c>
       <c r="F277" t="s">
-        <v>435</v>
+        <v>551</v>
       </c>
     </row>
     <row r="278" spans="1:6">
@@ -7639,7 +7659,7 @@
         <v>15</v>
       </c>
       <c r="F278" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
     </row>
     <row r="279" spans="1:6">
@@ -7659,7 +7679,7 @@
         <v>15</v>
       </c>
       <c r="F279" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
     </row>
     <row r="280" spans="1:6">
@@ -7679,7 +7699,7 @@
         <v>15</v>
       </c>
       <c r="F280" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
     </row>
     <row r="281" spans="1:6">
@@ -7699,7 +7719,7 @@
         <v>15</v>
       </c>
       <c r="F281" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
     </row>
     <row r="282" spans="1:6">
@@ -7719,7 +7739,7 @@
         <v>15</v>
       </c>
       <c r="F282" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
     </row>
     <row r="283" spans="1:6">
@@ -7739,7 +7759,7 @@
         <v>15</v>
       </c>
       <c r="F283" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
     </row>
     <row r="284" spans="1:6">
@@ -7759,7 +7779,7 @@
         <v>15</v>
       </c>
       <c r="F284" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
     </row>
     <row r="285" spans="1:6">
@@ -7779,7 +7799,7 @@
         <v>15</v>
       </c>
       <c r="F285" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
     </row>
     <row r="286" spans="1:6">
@@ -7799,7 +7819,7 @@
         <v>15</v>
       </c>
       <c r="F286" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
     </row>
     <row r="287" spans="1:6">
@@ -7819,7 +7839,7 @@
         <v>15</v>
       </c>
       <c r="F287" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
     </row>
     <row r="288" spans="1:6">
@@ -7839,7 +7859,7 @@
         <v>15</v>
       </c>
       <c r="F288" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
     </row>
     <row r="289" spans="1:6">
@@ -7859,7 +7879,7 @@
         <v>15</v>
       </c>
       <c r="F289" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
     </row>
     <row r="290" spans="1:6">
@@ -7879,7 +7899,7 @@
         <v>15</v>
       </c>
       <c r="F290" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
     </row>
     <row r="291" spans="1:6">
@@ -7899,7 +7919,7 @@
         <v>15</v>
       </c>
       <c r="F291" t="s">
-        <v>449</v>
+        <v>439</v>
       </c>
     </row>
     <row r="292" spans="1:6">
@@ -7919,7 +7939,7 @@
         <v>15</v>
       </c>
       <c r="F292" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
     </row>
     <row r="293" spans="1:6">
@@ -7939,7 +7959,7 @@
         <v>15</v>
       </c>
       <c r="F293" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
     </row>
     <row r="294" spans="1:6">
@@ -7959,7 +7979,7 @@
         <v>15</v>
       </c>
       <c r="F294" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
     </row>
     <row r="295" spans="1:6">
@@ -8999,7 +9019,7 @@
         <v>16</v>
       </c>
       <c r="F346" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
     </row>
     <row r="347" spans="1:6">
@@ -9019,7 +9039,7 @@
         <v>16</v>
       </c>
       <c r="F347" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
     </row>
     <row r="348" spans="1:6">
@@ -9039,7 +9059,7 @@
         <v>16</v>
       </c>
       <c r="F348" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
     </row>
     <row r="349" spans="1:6">
@@ -9059,7 +9079,7 @@
         <v>16</v>
       </c>
       <c r="F349" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
     </row>
     <row r="350" spans="1:6">
@@ -9079,7 +9099,7 @@
         <v>16</v>
       </c>
       <c r="F350" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
     </row>
     <row r="351" spans="1:6">
@@ -9099,7 +9119,7 @@
         <v>16</v>
       </c>
       <c r="F351" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
     </row>
     <row r="352" spans="1:6">
@@ -9119,7 +9139,7 @@
         <v>16</v>
       </c>
       <c r="F352" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
     </row>
     <row r="353" spans="1:6">
@@ -9139,7 +9159,7 @@
         <v>16</v>
       </c>
       <c r="F353" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
     </row>
     <row r="354" spans="1:6">
@@ -9159,7 +9179,7 @@
         <v>16</v>
       </c>
       <c r="F354" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
     </row>
     <row r="355" spans="1:6">
@@ -9179,7 +9199,7 @@
         <v>16</v>
       </c>
       <c r="F355" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
     </row>
     <row r="356" spans="1:6">
@@ -9199,7 +9219,7 @@
         <v>16</v>
       </c>
       <c r="F356" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
     </row>
     <row r="357" spans="1:6">
@@ -9219,7 +9239,7 @@
         <v>16</v>
       </c>
       <c r="F357" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
     </row>
     <row r="358" spans="1:6">
@@ -9239,7 +9259,7 @@
         <v>16</v>
       </c>
       <c r="F358" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
     </row>
     <row r="359" spans="1:6">
@@ -9259,7 +9279,7 @@
         <v>16</v>
       </c>
       <c r="F359" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
     </row>
     <row r="360" spans="1:6">
@@ -9279,7 +9299,7 @@
         <v>16</v>
       </c>
       <c r="F360" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="361" spans="1:6">
@@ -10959,7 +10979,7 @@
         <v>15</v>
       </c>
       <c r="F444" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
     </row>
     <row r="445" spans="1:6">
@@ -10979,7 +10999,7 @@
         <v>15</v>
       </c>
       <c r="F445" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
     </row>
     <row r="446" spans="1:6">
@@ -10999,7 +11019,7 @@
         <v>15</v>
       </c>
       <c r="F446" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
     </row>
     <row r="447" spans="1:6">
@@ -11019,7 +11039,7 @@
         <v>15</v>
       </c>
       <c r="F447" t="s">
-        <v>470</v>
+        <v>560</v>
       </c>
     </row>
     <row r="448" spans="1:6">
@@ -11039,7 +11059,7 @@
         <v>15</v>
       </c>
       <c r="F448" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
     </row>
     <row r="449" spans="1:6">
@@ -11059,7 +11079,7 @@
         <v>15</v>
       </c>
       <c r="F449" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
     </row>
     <row r="450" spans="1:6">
@@ -11079,7 +11099,7 @@
         <v>15</v>
       </c>
       <c r="F450" t="s">
-        <v>472</v>
+        <v>461</v>
       </c>
     </row>
     <row r="451" spans="1:6">
@@ -11099,7 +11119,7 @@
         <v>15</v>
       </c>
       <c r="F451" t="s">
-        <v>474</v>
+        <v>463</v>
       </c>
     </row>
     <row r="452" spans="1:6">
@@ -11119,7 +11139,7 @@
         <v>15</v>
       </c>
       <c r="F452" t="s">
-        <v>475</v>
+        <v>464</v>
       </c>
     </row>
     <row r="453" spans="1:6">
@@ -11539,7 +11559,7 @@
         <v>15</v>
       </c>
       <c r="F473" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
     </row>
     <row r="474" spans="1:6">
@@ -11559,7 +11579,7 @@
         <v>16</v>
       </c>
       <c r="F474" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
     </row>
     <row r="475" spans="1:6">
@@ -11579,7 +11599,7 @@
         <v>16</v>
       </c>
       <c r="F475" t="s">
-        <v>496</v>
+        <v>485</v>
       </c>
     </row>
     <row r="476" spans="1:6">
@@ -11599,7 +11619,7 @@
         <v>16</v>
       </c>
       <c r="F476" t="s">
-        <v>497</v>
+        <v>486</v>
       </c>
     </row>
     <row r="477" spans="1:6">
@@ -11619,7 +11639,7 @@
         <v>16</v>
       </c>
       <c r="F477" t="s">
-        <v>498</v>
+        <v>487</v>
       </c>
     </row>
     <row r="478" spans="1:6">
@@ -11639,7 +11659,7 @@
         <v>16</v>
       </c>
       <c r="F478" t="s">
-        <v>499</v>
+        <v>488</v>
       </c>
     </row>
     <row r="479" spans="1:6">
@@ -11659,7 +11679,7 @@
         <v>16</v>
       </c>
       <c r="F479" t="s">
-        <v>543</v>
+        <v>532</v>
       </c>
     </row>
     <row r="480" spans="1:6">
@@ -11679,7 +11699,7 @@
         <v>16</v>
       </c>
       <c r="F480" t="s">
-        <v>549</v>
+        <v>538</v>
       </c>
     </row>
     <row r="481" spans="1:6">
@@ -11699,7 +11719,7 @@
         <v>16</v>
       </c>
       <c r="F481" t="s">
-        <v>544</v>
+        <v>533</v>
       </c>
     </row>
     <row r="482" spans="1:6">
@@ -11719,7 +11739,7 @@
         <v>16</v>
       </c>
       <c r="F482" t="s">
-        <v>545</v>
+        <v>534</v>
       </c>
     </row>
     <row r="483" spans="1:6">
@@ -11739,7 +11759,7 @@
         <v>16</v>
       </c>
       <c r="F483" t="s">
-        <v>548</v>
+        <v>537</v>
       </c>
     </row>
     <row r="484" spans="1:6">
@@ -11759,7 +11779,7 @@
         <v>16</v>
       </c>
       <c r="F484" t="s">
-        <v>541</v>
+        <v>530</v>
       </c>
     </row>
     <row r="485" spans="1:6">
@@ -11779,7 +11799,7 @@
         <v>16</v>
       </c>
       <c r="F485" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
     </row>
     <row r="486" spans="1:6">
@@ -11799,7 +11819,7 @@
         <v>16</v>
       </c>
       <c r="F486" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
     </row>
     <row r="487" spans="1:6">
@@ -11819,7 +11839,7 @@
         <v>16</v>
       </c>
       <c r="F487" t="s">
-        <v>506</v>
+        <v>495</v>
       </c>
     </row>
     <row r="488" spans="1:6">
@@ -11839,7 +11859,7 @@
         <v>16</v>
       </c>
       <c r="F488" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
     </row>
     <row r="489" spans="1:6">
@@ -11859,7 +11879,7 @@
         <v>16</v>
       </c>
       <c r="F489" t="s">
-        <v>511</v>
+        <v>500</v>
       </c>
     </row>
     <row r="490" spans="1:6">
@@ -11879,7 +11899,7 @@
         <v>16</v>
       </c>
       <c r="F490" t="s">
-        <v>547</v>
+        <v>536</v>
       </c>
     </row>
     <row r="491" spans="1:6">
@@ -11899,7 +11919,7 @@
         <v>16</v>
       </c>
       <c r="F491" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="492" spans="1:6">
@@ -11919,7 +11939,7 @@
         <v>16</v>
       </c>
       <c r="F492" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
     </row>
     <row r="493" spans="1:6">
@@ -11939,7 +11959,7 @@
         <v>16</v>
       </c>
       <c r="F493" t="s">
-        <v>540</v>
+        <v>529</v>
       </c>
     </row>
     <row r="494" spans="1:6">
@@ -11959,7 +11979,7 @@
         <v>16</v>
       </c>
       <c r="F494" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
     </row>
     <row r="495" spans="1:6">
@@ -11979,7 +11999,7 @@
         <v>16</v>
       </c>
       <c r="F495" t="s">
-        <v>542</v>
+        <v>531</v>
       </c>
     </row>
     <row r="496" spans="1:6">
@@ -11999,7 +12019,7 @@
         <v>16</v>
       </c>
       <c r="F496" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
     </row>
     <row r="497" spans="1:6">
@@ -12019,7 +12039,7 @@
         <v>16</v>
       </c>
       <c r="F497" t="s">
-        <v>515</v>
+        <v>504</v>
       </c>
     </row>
     <row r="498" spans="1:6">
@@ -12039,7 +12059,7 @@
         <v>16</v>
       </c>
       <c r="F498" t="s">
-        <v>519</v>
+        <v>508</v>
       </c>
     </row>
     <row r="499" spans="1:6">
@@ -12059,7 +12079,7 @@
         <v>16</v>
       </c>
       <c r="F499" t="s">
-        <v>520</v>
+        <v>509</v>
       </c>
     </row>
     <row r="500" spans="1:6">
@@ -12099,7 +12119,7 @@
         <v>16</v>
       </c>
       <c r="F501" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
     </row>
     <row r="502" spans="1:6">
@@ -12119,7 +12139,7 @@
         <v>16</v>
       </c>
       <c r="F502" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
     </row>
     <row r="503" spans="1:6">
@@ -12139,7 +12159,7 @@
         <v>16</v>
       </c>
       <c r="F503" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
     </row>
     <row r="504" spans="1:6">
@@ -12159,7 +12179,7 @@
         <v>16</v>
       </c>
       <c r="F504" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
     </row>
     <row r="505" spans="1:6">
@@ -12179,7 +12199,7 @@
         <v>16</v>
       </c>
       <c r="F505" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
     </row>
     <row r="506" spans="1:6">
@@ -12199,7 +12219,7 @@
         <v>16</v>
       </c>
       <c r="F506" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
     </row>
     <row r="507" spans="1:6">
@@ -12219,7 +12239,7 @@
         <v>16</v>
       </c>
       <c r="F507" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="508" spans="1:6">
@@ -12239,7 +12259,7 @@
         <v>16</v>
       </c>
       <c r="F508" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
     </row>
     <row r="509" spans="1:6">
@@ -12259,7 +12279,7 @@
         <v>16</v>
       </c>
       <c r="F509" t="s">
-        <v>509</v>
+        <v>498</v>
       </c>
     </row>
     <row r="510" spans="1:6">
@@ -12279,7 +12299,7 @@
         <v>16</v>
       </c>
       <c r="F510" t="s">
-        <v>510</v>
+        <v>499</v>
       </c>
     </row>
     <row r="511" spans="1:6">
@@ -12299,7 +12319,7 @@
         <v>16</v>
       </c>
       <c r="F511" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="512" spans="1:6">
@@ -12319,7 +12339,7 @@
         <v>16</v>
       </c>
       <c r="F512" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
     </row>
     <row r="513" spans="1:6">
@@ -12339,7 +12359,7 @@
         <v>16</v>
       </c>
       <c r="F513" t="s">
-        <v>516</v>
+        <v>505</v>
       </c>
     </row>
     <row r="514" spans="1:6">
@@ -12359,7 +12379,7 @@
         <v>16</v>
       </c>
       <c r="F514" t="s">
-        <v>517</v>
+        <v>506</v>
       </c>
     </row>
     <row r="515" spans="1:6">
@@ -12379,7 +12399,7 @@
         <v>16</v>
       </c>
       <c r="F515" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="516" spans="1:6">
@@ -12399,7 +12419,7 @@
         <v>16</v>
       </c>
       <c r="F516" t="s">
-        <v>518</v>
+        <v>507</v>
       </c>
     </row>
     <row r="517" spans="1:6">
@@ -12419,7 +12439,7 @@
         <v>16</v>
       </c>
       <c r="F517" t="s">
-        <v>521</v>
+        <v>510</v>
       </c>
     </row>
     <row r="518" spans="1:6">
@@ -12439,7 +12459,7 @@
         <v>16</v>
       </c>
       <c r="F518" t="s">
-        <v>537</v>
+        <v>526</v>
       </c>
     </row>
     <row r="519" spans="1:6">
@@ -12459,7 +12479,7 @@
         <v>16</v>
       </c>
       <c r="F519" t="s">
-        <v>538</v>
+        <v>527</v>
       </c>
     </row>
     <row r="520" spans="1:6">
@@ -12479,7 +12499,7 @@
         <v>16</v>
       </c>
       <c r="F520" t="s">
-        <v>478</v>
+        <v>467</v>
       </c>
     </row>
     <row r="521" spans="1:6">
@@ -12499,7 +12519,7 @@
         <v>16</v>
       </c>
       <c r="F521" t="s">
-        <v>480</v>
+        <v>469</v>
       </c>
     </row>
     <row r="522" spans="1:6">
@@ -12519,7 +12539,7 @@
         <v>16</v>
       </c>
       <c r="F522" t="s">
-        <v>481</v>
+        <v>470</v>
       </c>
     </row>
     <row r="523" spans="1:6">
@@ -12539,7 +12559,7 @@
         <v>16</v>
       </c>
       <c r="F523" t="s">
-        <v>479</v>
+        <v>468</v>
       </c>
     </row>
     <row r="524" spans="1:6">
@@ -12559,7 +12579,7 @@
         <v>16</v>
       </c>
       <c r="F524" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
     </row>
     <row r="525" spans="1:6">
@@ -12579,7 +12599,7 @@
         <v>16</v>
       </c>
       <c r="F525" t="s">
-        <v>476</v>
+        <v>465</v>
       </c>
     </row>
     <row r="526" spans="1:6">
@@ -12599,7 +12619,7 @@
         <v>16</v>
       </c>
       <c r="F526" t="s">
-        <v>539</v>
+        <v>528</v>
       </c>
     </row>
     <row r="527" spans="1:6">
@@ -12619,7 +12639,7 @@
         <v>16</v>
       </c>
       <c r="F527" t="s">
-        <v>477</v>
+        <v>466</v>
       </c>
     </row>
     <row r="528" spans="1:6">
@@ -12639,7 +12659,7 @@
         <v>16</v>
       </c>
       <c r="F528" t="s">
-        <v>482</v>
+        <v>471</v>
       </c>
     </row>
     <row r="529" spans="1:6">
@@ -12659,7 +12679,7 @@
         <v>16</v>
       </c>
       <c r="F529" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
     </row>
     <row r="530" spans="1:6">
@@ -12679,7 +12699,7 @@
         <v>16</v>
       </c>
       <c r="F530" t="s">
-        <v>484</v>
+        <v>473</v>
       </c>
     </row>
     <row r="531" spans="1:6">
@@ -12699,7 +12719,7 @@
         <v>16</v>
       </c>
       <c r="F531" t="s">
-        <v>487</v>
+        <v>476</v>
       </c>
     </row>
     <row r="532" spans="1:6">
@@ -12719,7 +12739,7 @@
         <v>16</v>
       </c>
       <c r="F532" t="s">
-        <v>490</v>
+        <v>479</v>
       </c>
     </row>
     <row r="533" spans="1:6">
@@ -12739,7 +12759,7 @@
         <v>16</v>
       </c>
       <c r="F533" t="s">
-        <v>485</v>
+        <v>474</v>
       </c>
     </row>
     <row r="534" spans="1:6">
@@ -12759,7 +12779,7 @@
         <v>16</v>
       </c>
       <c r="F534" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="535" spans="1:6">
@@ -12779,7 +12799,7 @@
         <v>16</v>
       </c>
       <c r="F535" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
     </row>
     <row r="536" spans="1:6">
@@ -12799,7 +12819,7 @@
         <v>16</v>
       </c>
       <c r="F536" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="537" spans="1:6">
@@ -12819,7 +12839,7 @@
         <v>16</v>
       </c>
       <c r="F537" t="s">
-        <v>486</v>
+        <v>475</v>
       </c>
     </row>
     <row r="538" spans="1:6">
@@ -12839,7 +12859,7 @@
         <v>16</v>
       </c>
       <c r="F538" t="s">
-        <v>488</v>
+        <v>477</v>
       </c>
     </row>
     <row r="539" spans="1:6">
@@ -12859,7 +12879,7 @@
         <v>16</v>
       </c>
       <c r="F539" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
     </row>
     <row r="540" spans="1:6">
@@ -12879,7 +12899,7 @@
         <v>16</v>
       </c>
       <c r="F540" t="s">
-        <v>535</v>
+        <v>524</v>
       </c>
     </row>
     <row r="541" spans="1:6">
@@ -12899,7 +12919,7 @@
         <v>16</v>
       </c>
       <c r="F541" t="s">
-        <v>560</v>
+        <v>549</v>
       </c>
     </row>
     <row r="542" spans="1:6">
@@ -12919,7 +12939,7 @@
         <v>16</v>
       </c>
       <c r="F542" t="s">
-        <v>559</v>
+        <v>548</v>
       </c>
     </row>
     <row r="543" spans="1:6">
@@ -12939,7 +12959,7 @@
         <v>16</v>
       </c>
       <c r="F543" t="s">
-        <v>551</v>
+        <v>540</v>
       </c>
     </row>
     <row r="544" spans="1:6">
@@ -12959,7 +12979,7 @@
         <v>16</v>
       </c>
       <c r="F544" t="s">
-        <v>555</v>
+        <v>544</v>
       </c>
     </row>
     <row r="545" spans="1:6">
@@ -12979,7 +12999,7 @@
         <v>16</v>
       </c>
       <c r="F545" t="s">
-        <v>558</v>
+        <v>547</v>
       </c>
     </row>
     <row r="546" spans="1:6">
@@ -12999,7 +13019,7 @@
         <v>16</v>
       </c>
       <c r="F546" t="s">
-        <v>556</v>
+        <v>545</v>
       </c>
     </row>
     <row r="547" spans="1:6">
@@ -13019,7 +13039,7 @@
         <v>16</v>
       </c>
       <c r="F547" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
     </row>
     <row r="548" spans="1:6">
@@ -13039,7 +13059,7 @@
         <v>16</v>
       </c>
       <c r="F548" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
     </row>
     <row r="549" spans="1:6">
@@ -13059,7 +13079,7 @@
         <v>16</v>
       </c>
       <c r="F549" t="s">
-        <v>528</v>
+        <v>517</v>
       </c>
     </row>
     <row r="550" spans="1:6">
@@ -13079,7 +13099,7 @@
         <v>16</v>
       </c>
       <c r="F550" t="s">
-        <v>529</v>
+        <v>518</v>
       </c>
     </row>
     <row r="551" spans="1:6">
@@ -13099,7 +13119,7 @@
         <v>16</v>
       </c>
       <c r="F551" t="s">
-        <v>553</v>
+        <v>542</v>
       </c>
     </row>
     <row r="552" spans="1:6">
@@ -13119,7 +13139,7 @@
         <v>16</v>
       </c>
       <c r="F552" t="s">
-        <v>557</v>
+        <v>546</v>
       </c>
     </row>
     <row r="553" spans="1:6">
@@ -13139,7 +13159,7 @@
         <v>16</v>
       </c>
       <c r="F553" t="s">
-        <v>522</v>
+        <v>511</v>
       </c>
     </row>
     <row r="554" spans="1:6">
@@ -13159,7 +13179,7 @@
         <v>16</v>
       </c>
       <c r="F554" t="s">
-        <v>523</v>
+        <v>512</v>
       </c>
     </row>
     <row r="555" spans="1:6">
@@ -13179,7 +13199,7 @@
         <v>16</v>
       </c>
       <c r="F555" t="s">
-        <v>524</v>
+        <v>513</v>
       </c>
     </row>
     <row r="556" spans="1:6">
@@ -13199,7 +13219,7 @@
         <v>16</v>
       </c>
       <c r="F556" t="s">
-        <v>525</v>
+        <v>514</v>
       </c>
     </row>
     <row r="557" spans="1:6">
@@ -13219,7 +13239,7 @@
         <v>16</v>
       </c>
       <c r="F557" t="s">
-        <v>530</v>
+        <v>519</v>
       </c>
     </row>
     <row r="558" spans="1:6">
@@ -13239,7 +13259,7 @@
         <v>16</v>
       </c>
       <c r="F558" t="s">
-        <v>531</v>
+        <v>520</v>
       </c>
     </row>
     <row r="559" spans="1:6">
@@ -13259,7 +13279,7 @@
         <v>16</v>
       </c>
       <c r="F559" t="s">
-        <v>552</v>
+        <v>541</v>
       </c>
     </row>
     <row r="560" spans="1:6">
@@ -13279,7 +13299,7 @@
         <v>16</v>
       </c>
       <c r="F560" t="s">
-        <v>550</v>
+        <v>539</v>
       </c>
     </row>
     <row r="561" spans="1:6">
@@ -13299,7 +13319,7 @@
         <v>16</v>
       </c>
       <c r="F561" t="s">
-        <v>554</v>
+        <v>543</v>
       </c>
     </row>
     <row r="562" spans="1:6">
@@ -13319,7 +13339,7 @@
         <v>16</v>
       </c>
       <c r="F562" t="s">
-        <v>533</v>
+        <v>522</v>
       </c>
     </row>
     <row r="563" spans="1:6">
@@ -13339,7 +13359,7 @@
         <v>16</v>
       </c>
       <c r="F563" t="s">
-        <v>532</v>
+        <v>521</v>
       </c>
     </row>
     <row r="564" spans="1:6">
@@ -13359,7 +13379,7 @@
         <v>16</v>
       </c>
       <c r="F564" t="s">
-        <v>534</v>
+        <v>523</v>
       </c>
     </row>
     <row r="565" spans="1:6">
@@ -13379,7 +13399,7 @@
         <v>16</v>
       </c>
       <c r="F565" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
     </row>
     <row r="566" spans="1:6">
@@ -13399,7 +13419,7 @@
         <v>16</v>
       </c>
       <c r="F566" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -13412,6 +13432,7 @@
     <sortCondition ref="F2:F566"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>